<commit_message>
add move block property json
</commit_message>
<xml_diff>
--- a/meta/convertScript/MapInfo.xlsx
+++ b/meta/convertScript/MapInfo.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\limys\Desktop\MapTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ys\exp\githubRepo\fsba\meta\convertScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF59357-7E2C-49DA-8934-C05C10ADE541}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="MapInfo" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2493" uniqueCount="1688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2493" uniqueCount="1689">
   <si>
     <t xml:space="preserve"> 남남주                 </t>
   </si>
@@ -5093,13 +5092,17 @@
   </si>
   <si>
     <t>#T______</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>placeholder</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5825,23 +5828,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -5877,23 +5863,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -6069,12 +6038,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F501"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A462" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E478" sqref="E478"/>
+      <pane ySplit="1" topLeftCell="A156" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F177" sqref="F177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -9611,7 +9580,7 @@
         <v>175</v>
       </c>
       <c r="B177" t="s">
-        <v>123</v>
+        <v>1688</v>
       </c>
       <c r="C177" t="s">
         <v>266</v>
@@ -16068,7 +16037,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F501" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:F501">
     <sortState ref="A2:F501">
       <sortCondition ref="A1:A501"/>
     </sortState>

</xml_diff>